<commit_message>
22 Apr 2020 World Covid Status Updates
Updated Master to WHO Situation Report 93
Added Ukraine and experimented with Cumulative Normal Case fit
Added Video 22 Apr 2020 World Covid Status
</commit_message>
<xml_diff>
--- a/Analyses/Provisional_Death_Counts_for_Coronavirus_Disease__COVID-19_.xlsx
+++ b/Analyses/Provisional_Death_Counts_for_Coronavirus_Disease__COVID-19_.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="142">
   <si>
     <t>Group</t>
   </si>
@@ -688,6 +688,9 @@
   </si>
   <si>
     <t>United States Covid Deaths</t>
+  </si>
+  <si>
+    <t>Percent of Deaths by age</t>
   </si>
 </sst>
 </file>
@@ -1460,7 +1463,7 @@
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="83">
+  <cellXfs count="84">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="33" borderId="10" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1687,6 +1690,7 @@
     <xf numFmtId="166" fontId="21" fillId="38" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="3" fontId="0" fillId="39" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="18" fillId="36" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
@@ -1709,7 +1713,7 @@
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="3" fontId="0" fillId="39" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="33" borderId="10" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="45">
     <cellStyle name="20% - Accent1" xfId="21" builtinId="30" customBuiltin="1"/>
@@ -2130,11 +2134,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="339796768"/>
-        <c:axId val="339794024"/>
+        <c:axId val="531306312"/>
+        <c:axId val="336886424"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="339796768"/>
+        <c:axId val="531306312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2191,12 +2195,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="339794024"/>
+        <c:crossAx val="336886424"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="339794024"/>
+        <c:axId val="336886424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2253,7 +2257,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="339796768"/>
+        <c:crossAx val="531306312"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5683,7 +5687,7 @@
   <dimension ref="A1:AC94"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="L7" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="O24" sqref="O24"/>
+      <selection activeCell="O9" sqref="O9:P20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -5706,19 +5710,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:29" ht="2.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="76" t="s">
+      <c r="A1" s="77" t="s">
         <v>133</v>
       </c>
-      <c r="B1" s="76"/>
-      <c r="C1" s="76"/>
-      <c r="D1" s="76"/>
-      <c r="E1" s="76"/>
-      <c r="F1" s="76"/>
-      <c r="G1" s="76"/>
-      <c r="H1" s="76"/>
-      <c r="I1" s="76"/>
-      <c r="J1" s="76"/>
-      <c r="K1" s="76"/>
+      <c r="B1" s="77"/>
+      <c r="C1" s="77"/>
+      <c r="D1" s="77"/>
+      <c r="E1" s="77"/>
+      <c r="F1" s="77"/>
+      <c r="G1" s="77"/>
+      <c r="H1" s="77"/>
+      <c r="I1" s="77"/>
+      <c r="J1" s="77"/>
+      <c r="K1" s="77"/>
     </row>
     <row r="2" spans="1:29" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="45" t="s">
@@ -5859,10 +5863,10 @@
       <c r="L6" s="15"/>
       <c r="M6" s="15"/>
       <c r="P6" s="15"/>
-      <c r="Q6" s="81" t="s">
+      <c r="Q6" s="82" t="s">
         <v>136</v>
       </c>
-      <c r="R6" s="81"/>
+      <c r="R6" s="82"/>
       <c r="S6" s="54"/>
       <c r="T6" s="54"/>
       <c r="U6" s="54"/>
@@ -6001,7 +6005,9 @@
       <c r="I9" s="40"/>
       <c r="J9" s="40"/>
       <c r="K9" s="41"/>
-      <c r="L9" s="15"/>
+      <c r="L9" s="15" t="s">
+        <v>141</v>
+      </c>
       <c r="M9" s="15"/>
       <c r="N9" s="64" t="s">
         <v>136</v>
@@ -6065,10 +6071,13 @@
       <c r="J10" s="27">
         <v>21914</v>
       </c>
-      <c r="K10" s="28">
+      <c r="K10" s="27">
         <v>22144</v>
       </c>
-      <c r="L10" s="15"/>
+      <c r="L10" s="83">
+        <f>+N10/$N$21</f>
+        <v>0</v>
+      </c>
       <c r="M10" s="15" t="s">
         <v>17</v>
       </c>
@@ -6143,7 +6152,10 @@
       <c r="K11" s="28">
         <v>22261</v>
       </c>
-      <c r="L11" s="15"/>
+      <c r="L11" s="83">
+        <f t="shared" ref="L11:L20" si="3">+N11/$N$21</f>
+        <v>2.0659022828220226E-4</v>
+      </c>
       <c r="M11" s="15" t="s">
         <v>18</v>
       </c>
@@ -6155,7 +6167,7 @@
         <v>16351200</v>
       </c>
       <c r="P11" s="67">
-        <f t="shared" ref="P11:P20" si="3">1000000*(N11/O11)</f>
+        <f t="shared" ref="P11:P20" si="4">1000000*(N11/O11)</f>
         <v>0.1223151817603601</v>
       </c>
       <c r="Q11" s="69">
@@ -6218,7 +6230,10 @@
       <c r="K12" s="28">
         <v>22288</v>
       </c>
-      <c r="L12" s="15"/>
+      <c r="L12" s="83">
+        <f t="shared" si="3"/>
+        <v>1.0329511414110113E-4</v>
+      </c>
       <c r="M12" s="15" t="s">
         <v>19</v>
       </c>
@@ -6230,7 +6245,7 @@
         <v>40970000</v>
       </c>
       <c r="P12" s="67">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2.4408103490358799E-2</v>
       </c>
       <c r="Q12" s="69">
@@ -6293,7 +6308,10 @@
       <c r="K13" s="28">
         <v>22527</v>
       </c>
-      <c r="L13" s="15"/>
+      <c r="L13" s="83">
+        <f t="shared" si="3"/>
+        <v>9.2965602726991013E-4</v>
+      </c>
       <c r="M13" s="15" t="s">
         <v>20</v>
       </c>
@@ -6305,7 +6323,7 @@
         <v>42937000</v>
       </c>
       <c r="P13" s="67">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.20960942776626221</v>
       </c>
       <c r="Q13" s="69">
@@ -6368,7 +6386,10 @@
       <c r="K14" s="28">
         <v>23384</v>
       </c>
-      <c r="L14" s="15"/>
+      <c r="L14" s="83">
+        <f t="shared" si="3"/>
+        <v>9.2965602726991017E-3</v>
+      </c>
       <c r="M14" s="15" t="s">
         <v>21</v>
       </c>
@@ -6380,7 +6401,7 @@
         <v>46491000</v>
       </c>
       <c r="P14" s="67">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1.9358585532683745</v>
       </c>
       <c r="Q14" s="69">
@@ -6443,7 +6464,10 @@
       <c r="K15" s="28">
         <v>24387</v>
       </c>
-      <c r="L15" s="15"/>
+      <c r="L15" s="83">
+        <f t="shared" si="3"/>
+        <v>2.2415039768618944E-2</v>
+      </c>
       <c r="M15" s="15" t="s">
         <v>22</v>
       </c>
@@ -6455,7 +6479,7 @@
         <v>42352000</v>
       </c>
       <c r="P15" s="67">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>5.1237249716660367</v>
       </c>
       <c r="Q15" s="69">
@@ -6518,7 +6542,10 @@
       <c r="K16" s="28">
         <v>25155</v>
       </c>
-      <c r="L16" s="15"/>
+      <c r="L16" s="83">
+        <f t="shared" si="3"/>
+        <v>5.7638673690734429E-2</v>
+      </c>
       <c r="M16" s="15" t="s">
         <v>23</v>
       </c>
@@ -6530,7 +6557,7 @@
         <v>40615000</v>
       </c>
       <c r="P16" s="67">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>13.738766465591532</v>
       </c>
       <c r="Q16" s="69">
@@ -6593,7 +6620,10 @@
       <c r="K17" s="28">
         <v>25470</v>
       </c>
-      <c r="L17" s="15"/>
+      <c r="L17" s="83">
+        <f t="shared" si="3"/>
+        <v>0.13128809007333953</v>
+      </c>
       <c r="M17" s="15" t="s">
         <v>24</v>
       </c>
@@ -6605,7 +6635,7 @@
         <v>42783000</v>
       </c>
       <c r="P17" s="67">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>29.708061613257602</v>
       </c>
       <c r="Q17" s="69">
@@ -6668,7 +6698,10 @@
       <c r="K18" s="28">
         <v>25218</v>
       </c>
-      <c r="L18" s="15"/>
+      <c r="L18" s="83">
+        <f t="shared" si="3"/>
+        <v>0.22229108563164962</v>
+      </c>
       <c r="M18" s="15" t="s">
         <v>25</v>
       </c>
@@ -6680,7 +6713,7 @@
         <v>32789000</v>
       </c>
       <c r="P18" s="67">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>65.631766751044552</v>
       </c>
       <c r="Q18" s="69">
@@ -6743,7 +6776,10 @@
       <c r="K19" s="28">
         <v>24680</v>
       </c>
-      <c r="L19" s="15"/>
+      <c r="L19" s="83">
+        <f t="shared" si="3"/>
+        <v>0.27114967462039047</v>
+      </c>
       <c r="M19" s="15" t="s">
         <v>26</v>
       </c>
@@ -6755,7 +6791,7 @@
         <v>16561000</v>
       </c>
       <c r="P19" s="67">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>158.50492120041062</v>
       </c>
       <c r="Q19" s="69">
@@ -6818,7 +6854,10 @@
       <c r="K20" s="28">
         <v>24681</v>
       </c>
-      <c r="L20" s="15"/>
+      <c r="L20" s="83">
+        <f t="shared" si="3"/>
+        <v>0.2846813345728747</v>
+      </c>
       <c r="M20" s="15" t="s">
         <v>27</v>
       </c>
@@ -6830,7 +6869,7 @@
         <v>6701000</v>
       </c>
       <c r="P20" s="67">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>411.28189822414566</v>
       </c>
       <c r="Q20" s="69">
@@ -6895,7 +6934,7 @@
       </c>
       <c r="L21" s="15"/>
       <c r="M21" s="15"/>
-      <c r="N21" s="82">
+      <c r="N21" s="76">
         <f>+S7+T7</f>
         <v>9681</v>
       </c>
@@ -9328,19 +9367,19 @@
       <c r="AC81" s="54"/>
     </row>
     <row r="82" spans="1:29" s="21" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A82" s="77" t="s">
+      <c r="A82" s="78" t="s">
         <v>102</v>
       </c>
-      <c r="B82" s="78"/>
-      <c r="C82" s="78"/>
-      <c r="D82" s="78"/>
-      <c r="E82" s="78"/>
-      <c r="F82" s="78"/>
-      <c r="G82" s="78"/>
-      <c r="H82" s="78"/>
-      <c r="I82" s="78"/>
-      <c r="J82" s="78"/>
-      <c r="K82" s="78"/>
+      <c r="B82" s="79"/>
+      <c r="C82" s="79"/>
+      <c r="D82" s="79"/>
+      <c r="E82" s="79"/>
+      <c r="F82" s="79"/>
+      <c r="G82" s="79"/>
+      <c r="H82" s="79"/>
+      <c r="I82" s="79"/>
+      <c r="J82" s="79"/>
+      <c r="K82" s="79"/>
       <c r="Q82" s="54"/>
       <c r="R82" s="54"/>
       <c r="S82" s="54"/>
@@ -9383,83 +9422,83 @@
       </c>
     </row>
     <row r="88" spans="1:29" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A88" s="79" t="s">
+      <c r="A88" s="80" t="s">
         <v>98</v>
       </c>
-      <c r="B88" s="80"/>
-      <c r="C88" s="80"/>
-      <c r="D88" s="80"/>
-      <c r="E88" s="80"/>
-      <c r="F88" s="80"/>
-      <c r="G88" s="80"/>
-      <c r="H88" s="80"/>
-      <c r="I88" s="78"/>
+      <c r="B88" s="81"/>
+      <c r="C88" s="81"/>
+      <c r="D88" s="81"/>
+      <c r="E88" s="81"/>
+      <c r="F88" s="81"/>
+      <c r="G88" s="81"/>
+      <c r="H88" s="81"/>
+      <c r="I88" s="79"/>
     </row>
     <row r="89" spans="1:29" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A89" s="79"/>
-      <c r="B89" s="80"/>
-      <c r="C89" s="80"/>
-      <c r="D89" s="80"/>
-      <c r="E89" s="80"/>
-      <c r="F89" s="80"/>
-      <c r="G89" s="80"/>
-      <c r="H89" s="80"/>
-      <c r="I89" s="78"/>
+      <c r="A89" s="80"/>
+      <c r="B89" s="81"/>
+      <c r="C89" s="81"/>
+      <c r="D89" s="81"/>
+      <c r="E89" s="81"/>
+      <c r="F89" s="81"/>
+      <c r="G89" s="81"/>
+      <c r="H89" s="81"/>
+      <c r="I89" s="79"/>
     </row>
     <row r="90" spans="1:29" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A90" s="79"/>
-      <c r="B90" s="80"/>
-      <c r="C90" s="80"/>
-      <c r="D90" s="80"/>
-      <c r="E90" s="80"/>
-      <c r="F90" s="80"/>
-      <c r="G90" s="80"/>
-      <c r="H90" s="80"/>
-      <c r="I90" s="78"/>
+      <c r="A90" s="80"/>
+      <c r="B90" s="81"/>
+      <c r="C90" s="81"/>
+      <c r="D90" s="81"/>
+      <c r="E90" s="81"/>
+      <c r="F90" s="81"/>
+      <c r="G90" s="81"/>
+      <c r="H90" s="81"/>
+      <c r="I90" s="79"/>
     </row>
     <row r="91" spans="1:29" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A91" s="79"/>
-      <c r="B91" s="80"/>
-      <c r="C91" s="80"/>
-      <c r="D91" s="80"/>
-      <c r="E91" s="80"/>
-      <c r="F91" s="80"/>
-      <c r="G91" s="80"/>
-      <c r="H91" s="80"/>
-      <c r="I91" s="78"/>
+      <c r="A91" s="80"/>
+      <c r="B91" s="81"/>
+      <c r="C91" s="81"/>
+      <c r="D91" s="81"/>
+      <c r="E91" s="81"/>
+      <c r="F91" s="81"/>
+      <c r="G91" s="81"/>
+      <c r="H91" s="81"/>
+      <c r="I91" s="79"/>
     </row>
     <row r="92" spans="1:29" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A92" s="79"/>
-      <c r="B92" s="80"/>
-      <c r="C92" s="80"/>
-      <c r="D92" s="80"/>
-      <c r="E92" s="80"/>
-      <c r="F92" s="80"/>
-      <c r="G92" s="80"/>
-      <c r="H92" s="80"/>
-      <c r="I92" s="78"/>
+      <c r="A92" s="80"/>
+      <c r="B92" s="81"/>
+      <c r="C92" s="81"/>
+      <c r="D92" s="81"/>
+      <c r="E92" s="81"/>
+      <c r="F92" s="81"/>
+      <c r="G92" s="81"/>
+      <c r="H92" s="81"/>
+      <c r="I92" s="79"/>
     </row>
     <row r="93" spans="1:29" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A93" s="80"/>
-      <c r="B93" s="80"/>
-      <c r="C93" s="80"/>
-      <c r="D93" s="80"/>
-      <c r="E93" s="80"/>
-      <c r="F93" s="80"/>
-      <c r="G93" s="80"/>
-      <c r="H93" s="80"/>
-      <c r="I93" s="78"/>
+      <c r="A93" s="81"/>
+      <c r="B93" s="81"/>
+      <c r="C93" s="81"/>
+      <c r="D93" s="81"/>
+      <c r="E93" s="81"/>
+      <c r="F93" s="81"/>
+      <c r="G93" s="81"/>
+      <c r="H93" s="81"/>
+      <c r="I93" s="79"/>
     </row>
     <row r="94" spans="1:29" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A94" s="80"/>
-      <c r="B94" s="80"/>
-      <c r="C94" s="80"/>
-      <c r="D94" s="80"/>
-      <c r="E94" s="80"/>
-      <c r="F94" s="80"/>
-      <c r="G94" s="80"/>
-      <c r="H94" s="80"/>
-      <c r="I94" s="78"/>
+      <c r="A94" s="81"/>
+      <c r="B94" s="81"/>
+      <c r="C94" s="81"/>
+      <c r="D94" s="81"/>
+      <c r="E94" s="81"/>
+      <c r="F94" s="81"/>
+      <c r="G94" s="81"/>
+      <c r="H94" s="81"/>
+      <c r="I94" s="79"/>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>

<commit_message>
26 Apr 2020 Several Days of updated spreadsheets for videos
I am slowly reviewing as many data sites as I can.  I put notes now at www.SystemicIssues.Org with a grading system for sites.  The grade is on effectiveness in using technology and internet tools
</commit_message>
<xml_diff>
--- a/Analyses/Provisional_Death_Counts_for_Coronavirus_Disease__COVID-19_.xlsx
+++ b/Analyses/Provisional_Death_Counts_for_Coronavirus_Disease__COVID-19_.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="143">
   <si>
     <t>Group</t>
   </si>
@@ -691,6 +691,9 @@
   </si>
   <si>
     <t>Percent of Deaths by age</t>
+  </si>
+  <si>
+    <t>Covid Death Rates per Million</t>
   </si>
 </sst>
 </file>
@@ -1463,7 +1466,7 @@
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="84">
+  <cellXfs count="87">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="33" borderId="10" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1695,6 +1698,14 @@
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="33" borderId="10" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="36" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment wrapText="1"/>
       <protection locked="0"/>
@@ -1713,7 +1724,10 @@
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="10" fontId="0" fillId="33" borderId="10" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
   </cellXfs>
   <cellStyles count="45">
     <cellStyle name="20% - Accent1" xfId="21" builtinId="30" customBuiltin="1"/>
@@ -1868,7 +1882,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Main series'!$V$9</c:f>
+              <c:f>'Main series'!$W$9</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1903,7 +1917,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'Main series'!$U$10:$U$20</c:f>
+              <c:f>'Main series'!$P$10:$P$20</c:f>
               <c:numCache>
                 <c:formatCode>_(* #,##0.0_);_(* \(#,##0.0\);_(* "-"??_);_(@_)</c:formatCode>
                 <c:ptCount val="11"/>
@@ -1945,7 +1959,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Main series'!$V$10:$V$20</c:f>
+              <c:f>'Main series'!$W$10:$W$20</c:f>
               <c:numCache>
                 <c:formatCode>_(* #,##0.00_);_(* \(#,##0.00\);_(* "-"??_);_(@_)</c:formatCode>
                 <c:ptCount val="11"/>
@@ -1992,7 +2006,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Main series'!$W$9</c:f>
+              <c:f>'Main series'!$X$9</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2042,7 +2056,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>'Main series'!$U$10:$U$20</c:f>
+              <c:f>'Main series'!$P$10:$P$20</c:f>
               <c:numCache>
                 <c:formatCode>_(* #,##0.0_);_(* \(#,##0.0\);_(* "-"??_);_(@_)</c:formatCode>
                 <c:ptCount val="11"/>
@@ -2084,7 +2098,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Main series'!$W$10:$W$20</c:f>
+              <c:f>'Main series'!$X$10:$X$20</c:f>
               <c:numCache>
                 <c:formatCode>_(* #,##0.00_);_(* \(#,##0.00\);_(* "-"??_);_(@_)</c:formatCode>
                 <c:ptCount val="11"/>
@@ -2134,11 +2148,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="531306312"/>
-        <c:axId val="336886424"/>
+        <c:axId val="251737400"/>
+        <c:axId val="251737792"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="531306312"/>
+        <c:axId val="251737400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2195,12 +2209,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="336886424"/>
+        <c:crossAx val="251737792"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="336886424"/>
+        <c:axId val="251737792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2257,7 +2271,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="531306312"/>
+        <c:crossAx val="251737400"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2338,7 +2352,432 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>US Population by</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> Age</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Main series'!$Q$9</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Population</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Main series'!$P$10:$P$20</c:f>
+              <c:numCache>
+                <c:formatCode>_(* #,##0.0_);_(* \(#,##0.0\);_(* "-"??_);_(@_)</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>90</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Main series'!$Q$10:$Q$20</c:f>
+              <c:numCache>
+                <c:formatCode>_(* #,##0_);_(* \(#,##0\);_(* "-"??_);_(@_)</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>4087800</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>16351200</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>40970000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>42937000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>46491000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>42352000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>40615000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>42783000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>32789000</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>16561000</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>6701000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="414172016"/>
+        <c:axId val="414171624"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="414172016"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="_(* #,##0.0_);_(* \(#,##0.0\);_(* &quot;-&quot;??_);_(@_)" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="414171624"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="414171624"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="414172016"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -2894,20 +3333,536 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>658586</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>35378</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>92529</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>57149</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>582386</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>65314</xdr:rowOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>272143</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>87085</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2921,6 +3876,36 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>590550</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>27215</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>476250</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>122463</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -5684,47 +6669,48 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AC94"/>
+  <dimension ref="A1:AD94"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L7" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="O9" sqref="O9:P20"/>
+    <sheetView tabSelected="1" topLeftCell="M7" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="W7" sqref="W7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20.6640625" style="16" customWidth="1"/>
-    <col min="2" max="11" width="10.6640625" style="16" customWidth="1"/>
-    <col min="12" max="12" width="9.109375" style="16"/>
-    <col min="13" max="13" width="15.44140625" style="16" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="9.109375" style="16"/>
-    <col min="15" max="15" width="11.33203125" style="16" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="16.5546875" style="16" bestFit="1" customWidth="1"/>
-    <col min="17" max="18" width="9.44140625" style="54" bestFit="1" customWidth="1"/>
-    <col min="19" max="20" width="10.44140625" style="54" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="10.44140625" style="54" customWidth="1"/>
-    <col min="22" max="22" width="11.88671875" style="54" customWidth="1"/>
-    <col min="23" max="23" width="13.33203125" style="54" customWidth="1"/>
-    <col min="24" max="24" width="13.109375" style="54" customWidth="1"/>
-    <col min="25" max="29" width="9.109375" style="54"/>
-    <col min="30" max="16384" width="9.109375" style="16"/>
+    <col min="2" max="12" width="10.6640625" style="16" customWidth="1"/>
+    <col min="13" max="13" width="9.109375" style="16"/>
+    <col min="14" max="14" width="15.44140625" style="16" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9.109375" style="16"/>
+    <col min="16" max="16" width="10.44140625" style="54" customWidth="1"/>
+    <col min="17" max="17" width="11.33203125" style="16" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="16.5546875" style="16" bestFit="1" customWidth="1"/>
+    <col min="19" max="20" width="9.44140625" style="54" bestFit="1" customWidth="1"/>
+    <col min="21" max="22" width="10.44140625" style="54" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="11.88671875" style="54" customWidth="1"/>
+    <col min="24" max="24" width="13.33203125" style="54" customWidth="1"/>
+    <col min="25" max="25" width="13.109375" style="54" customWidth="1"/>
+    <col min="26" max="30" width="9.109375" style="54"/>
+    <col min="31" max="16384" width="9.109375" style="16"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" ht="2.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="77" t="s">
+    <row r="1" spans="1:30" ht="2.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="80" t="s">
         <v>133</v>
       </c>
-      <c r="B1" s="77"/>
-      <c r="C1" s="77"/>
-      <c r="D1" s="77"/>
-      <c r="E1" s="77"/>
-      <c r="F1" s="77"/>
-      <c r="G1" s="77"/>
-      <c r="H1" s="77"/>
-      <c r="I1" s="77"/>
-      <c r="J1" s="77"/>
-      <c r="K1" s="77"/>
-    </row>
-    <row r="2" spans="1:29" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="80"/>
+      <c r="C1" s="80"/>
+      <c r="D1" s="80"/>
+      <c r="E1" s="80"/>
+      <c r="F1" s="80"/>
+      <c r="G1" s="80"/>
+      <c r="H1" s="80"/>
+      <c r="I1" s="80"/>
+      <c r="J1" s="80"/>
+      <c r="K1" s="80"/>
+      <c r="L1" s="77"/>
+    </row>
+    <row r="2" spans="1:30" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="45" t="s">
         <v>132</v>
       </c>
@@ -5738,15 +6724,16 @@
       <c r="I2" s="24"/>
       <c r="J2" s="24"/>
       <c r="K2" s="24"/>
-      <c r="L2" s="26"/>
+      <c r="L2" s="24"/>
       <c r="M2" s="26"/>
       <c r="N2" s="26"/>
       <c r="O2" s="26"/>
-      <c r="P2" s="26" t="s">
+      <c r="Q2" s="26"/>
+      <c r="R2" s="26" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="3" spans="1:29" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:30" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="44" t="s">
         <v>131</v>
       </c>
@@ -5760,15 +6747,16 @@
       <c r="I3" s="24"/>
       <c r="J3" s="24"/>
       <c r="K3" s="24"/>
-      <c r="L3" s="26"/>
+      <c r="L3" s="24"/>
       <c r="M3" s="26"/>
       <c r="N3" s="26"/>
       <c r="O3" s="26"/>
-      <c r="Q3" s="16"/>
-      <c r="R3" s="16"/>
+      <c r="Q3" s="26"/>
       <c r="S3" s="16"/>
-    </row>
-    <row r="4" spans="1:29" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="T3" s="16"/>
+      <c r="U3" s="16"/>
+    </row>
+    <row r="4" spans="1:30" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="44" t="s">
         <v>130</v>
       </c>
@@ -5782,20 +6770,21 @@
       <c r="I4" s="24"/>
       <c r="J4" s="24"/>
       <c r="K4" s="24"/>
-      <c r="L4" s="26"/>
+      <c r="L4" s="24"/>
       <c r="M4" s="26"/>
       <c r="N4" s="26"/>
       <c r="O4" s="26"/>
-      <c r="Q4" s="68">
-        <f>SUM(Q10:Q20)</f>
+      <c r="Q4" s="26"/>
+      <c r="S4" s="68">
+        <f>SUM(S10:S20)</f>
         <v>3931</v>
       </c>
-      <c r="R4" s="68">
-        <f>SUM(R10:R20)</f>
+      <c r="T4" s="68">
+        <f>SUM(T10:T20)</f>
         <v>5750.0000000000009</v>
       </c>
     </row>
-    <row r="5" spans="1:29" s="17" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:30" s="17" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="24" t="s">
         <v>129</v>
       </c>
@@ -5809,9 +6798,9 @@
       <c r="I5" s="23"/>
       <c r="J5" s="23"/>
       <c r="K5" s="25"/>
-      <c r="L5" s="26"/>
+      <c r="L5" s="25"/>
       <c r="M5" s="26"/>
-      <c r="N5" s="54"/>
+      <c r="N5" s="26"/>
       <c r="O5" s="54"/>
       <c r="P5" s="54"/>
       <c r="Q5" s="54"/>
@@ -5827,8 +6816,9 @@
       <c r="AA5" s="54"/>
       <c r="AB5" s="54"/>
       <c r="AC5" s="54"/>
-    </row>
-    <row r="6" spans="1:29" s="18" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AD5" s="54"/>
+    </row>
+    <row r="6" spans="1:30" s="18" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="22"/>
       <c r="B6" s="55">
         <v>2016</v>
@@ -5860,26 +6850,29 @@
       <c r="K6" s="43">
         <v>2060</v>
       </c>
-      <c r="L6" s="15"/>
+      <c r="L6" s="86"/>
       <c r="M6" s="15"/>
-      <c r="P6" s="15"/>
-      <c r="Q6" s="82" t="s">
+      <c r="N6" s="15"/>
+      <c r="P6" s="54"/>
+      <c r="R6" s="15"/>
+      <c r="S6" s="85" t="s">
         <v>136</v>
       </c>
-      <c r="R6" s="82"/>
-      <c r="S6" s="54"/>
-      <c r="T6" s="54"/>
+      <c r="T6" s="85"/>
       <c r="U6" s="54"/>
       <c r="V6" s="54"/>
-      <c r="W6" s="54"/>
+      <c r="W6" s="54" t="s">
+        <v>142</v>
+      </c>
       <c r="X6" s="54"/>
       <c r="Y6" s="54"/>
       <c r="Z6" s="54"/>
       <c r="AA6" s="54"/>
       <c r="AB6" s="54"/>
       <c r="AC6" s="54"/>
-    </row>
-    <row r="7" spans="1:29" s="21" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AD6" s="54"/>
+    </row>
+    <row r="7" spans="1:30" s="21" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="33" t="s">
         <v>89</v>
       </c>
@@ -5913,44 +6906,45 @@
       <c r="K7" s="30">
         <v>404483</v>
       </c>
-      <c r="L7" s="15"/>
+      <c r="L7" s="29"/>
       <c r="M7" s="15"/>
-      <c r="N7" s="21" t="s">
+      <c r="N7" s="15"/>
+      <c r="O7" s="21" t="s">
         <v>140</v>
       </c>
-      <c r="O7" s="52"/>
-      <c r="P7" s="51"/>
-      <c r="Q7" s="70">
-        <f>+S7/$N$21</f>
+      <c r="P7" s="1"/>
+      <c r="Q7" s="52"/>
+      <c r="R7" s="51"/>
+      <c r="S7" s="70">
+        <f>+U7/$O$21</f>
         <v>0.40605309368866854</v>
       </c>
-      <c r="R7" s="70">
-        <f>+T7/$N$21</f>
+      <c r="T7" s="70">
+        <f>+V7/$O$21</f>
         <v>0.59394690631133151</v>
       </c>
-      <c r="S7" s="1">
+      <c r="U7" s="1">
         <v>3931</v>
       </c>
-      <c r="T7" s="1">
+      <c r="V7" s="1">
         <v>5750</v>
-      </c>
-      <c r="U7" s="1"/>
-      <c r="V7" s="14">
-        <f>SUM(V10:V20)</f>
-        <v>466.45546406596816</v>
       </c>
       <c r="W7" s="14">
         <f>SUM(W10:W20)</f>
+        <v>466.45546406596816</v>
+      </c>
+      <c r="X7" s="14">
+        <f>SUM(X10:X20)</f>
         <v>1036.6734118075024</v>
       </c>
-      <c r="X7" s="54"/>
       <c r="Y7" s="54"/>
       <c r="Z7" s="54"/>
       <c r="AA7" s="54"/>
       <c r="AB7" s="54"/>
       <c r="AC7" s="54"/>
-    </row>
-    <row r="8" spans="1:29" s="52" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AD7" s="54"/>
+    </row>
+    <row r="8" spans="1:30" s="52" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="48" t="s">
         <v>126</v>
       </c>
@@ -5984,16 +6978,17 @@
       <c r="K8" s="50">
         <v>42.88</v>
       </c>
-      <c r="L8" s="51"/>
+      <c r="L8" s="49"/>
       <c r="M8" s="51"/>
-      <c r="X8" s="54"/>
+      <c r="N8" s="51"/>
       <c r="Y8" s="54"/>
       <c r="Z8" s="54"/>
       <c r="AA8" s="54"/>
       <c r="AB8" s="54"/>
       <c r="AC8" s="54"/>
-    </row>
-    <row r="9" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AD8" s="54"/>
+    </row>
+    <row r="9" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="20"/>
       <c r="B9" s="58"/>
       <c r="C9" s="40"/>
@@ -6005,24 +7000,22 @@
       <c r="I9" s="40"/>
       <c r="J9" s="40"/>
       <c r="K9" s="41"/>
-      <c r="L9" s="15" t="s">
+      <c r="L9" s="40"/>
+      <c r="M9" s="15" t="s">
         <v>141</v>
       </c>
-      <c r="M9" s="15"/>
-      <c r="N9" s="64" t="s">
+      <c r="N9" s="15"/>
+      <c r="O9" s="64" t="s">
         <v>136</v>
       </c>
-      <c r="O9" s="64" t="s">
+      <c r="P9" s="65" t="s">
+        <v>139</v>
+      </c>
+      <c r="Q9" s="64" t="s">
         <v>135</v>
       </c>
-      <c r="P9" s="64" t="s">
+      <c r="R9" s="64" t="s">
         <v>137</v>
-      </c>
-      <c r="Q9" s="65" t="s">
-        <v>86</v>
-      </c>
-      <c r="R9" s="65" t="s">
-        <v>85</v>
       </c>
       <c r="S9" s="65" t="s">
         <v>86</v>
@@ -6031,16 +7024,19 @@
         <v>85</v>
       </c>
       <c r="U9" s="65" t="s">
-        <v>139</v>
+        <v>86</v>
       </c>
       <c r="V9" s="65" t="s">
+        <v>85</v>
+      </c>
+      <c r="W9" s="65" t="s">
         <v>86</v>
       </c>
-      <c r="W9" s="65" t="s">
+      <c r="X9" s="65" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="10" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="19" t="s">
         <v>125</v>
       </c>
@@ -6074,51 +7070,52 @@
       <c r="K10" s="27">
         <v>22144</v>
       </c>
-      <c r="L10" s="83">
-        <f>+N10/$N$21</f>
+      <c r="L10" s="27"/>
+      <c r="M10" s="79">
+        <f>+O10/$O$21</f>
         <v>0</v>
       </c>
-      <c r="M10" s="15" t="s">
+      <c r="N10" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="N10" s="63">
+      <c r="O10" s="63">
         <v>0</v>
       </c>
-      <c r="O10" s="66">
+      <c r="P10" s="74">
+        <v>0.2</v>
+      </c>
+      <c r="Q10" s="66">
         <f>1000*C10/5</f>
         <v>4087800</v>
       </c>
-      <c r="P10" s="67">
-        <f>1000000*(N10/O10)</f>
+      <c r="R10" s="67">
+        <f>1000000*(O10/Q10)</f>
         <v>0</v>
       </c>
-      <c r="Q10" s="69">
-        <f t="shared" ref="Q10:R20" si="0">+$N10*Q$7</f>
+      <c r="S10" s="69">
+        <f t="shared" ref="S10:T20" si="0">+$O10*S$7</f>
         <v>0</v>
       </c>
-      <c r="R10" s="69">
+      <c r="T10" s="69">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="S10" s="71">
+      <c r="U10" s="71">
         <v>1.9985999999999999</v>
       </c>
-      <c r="T10" s="71">
+      <c r="V10" s="71">
         <v>2.0891999999999999</v>
       </c>
-      <c r="U10" s="74">
-        <v>0.2</v>
-      </c>
-      <c r="V10" s="72">
-        <f t="shared" ref="V10:V20" si="1">+Q10/S10</f>
+      <c r="W10" s="72">
+        <f t="shared" ref="W10:W20" si="1">+S10/U10</f>
         <v>0</v>
       </c>
-      <c r="W10" s="72">
-        <f t="shared" ref="W10:W20" si="2">+R10/T10</f>
+      <c r="X10" s="72">
+        <f t="shared" ref="X10:X20" si="2">+T10/V10</f>
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="19" t="s">
         <v>124</v>
       </c>
@@ -6152,51 +7149,52 @@
       <c r="K11" s="28">
         <v>22261</v>
       </c>
-      <c r="L11" s="83">
-        <f t="shared" ref="L11:L20" si="3">+N11/$N$21</f>
+      <c r="L11" s="27"/>
+      <c r="M11" s="79">
+        <f t="shared" ref="M11:M20" si="3">+O11/$O$21</f>
         <v>2.0659022828220226E-4</v>
       </c>
-      <c r="M11" s="15" t="s">
+      <c r="N11" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="N11" s="4">
+      <c r="O11" s="4">
         <v>2</v>
       </c>
-      <c r="O11" s="66">
-        <f>1000*C10-O10</f>
+      <c r="P11" s="75">
+        <v>2</v>
+      </c>
+      <c r="Q11" s="66">
+        <f>1000*C10-Q10</f>
         <v>16351200</v>
       </c>
-      <c r="P11" s="67">
-        <f t="shared" ref="P11:P20" si="4">1000000*(N11/O11)</f>
+      <c r="R11" s="67">
+        <f t="shared" ref="R11:R20" si="4">1000000*(O11/Q11)</f>
         <v>0.1223151817603601</v>
       </c>
-      <c r="Q11" s="69">
+      <c r="S11" s="69">
         <f t="shared" si="0"/>
         <v>0.81210618737733709</v>
       </c>
-      <c r="R11" s="69">
+      <c r="T11" s="69">
         <f t="shared" si="0"/>
         <v>1.187893812622663</v>
       </c>
-      <c r="S11" s="71">
+      <c r="U11" s="71">
         <v>7.9943999999999997</v>
       </c>
-      <c r="T11" s="71">
+      <c r="V11" s="71">
         <v>8.3567999999999998</v>
       </c>
-      <c r="U11" s="75">
-        <v>2</v>
-      </c>
-      <c r="V11" s="73">
+      <c r="W11" s="73">
         <f t="shared" si="1"/>
         <v>0.10158438248991007</v>
       </c>
-      <c r="W11" s="73">
+      <c r="X11" s="73">
         <f t="shared" si="2"/>
         <v>0.14214697164257409</v>
       </c>
     </row>
-    <row r="12" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="19" t="s">
         <v>123</v>
       </c>
@@ -6230,51 +7228,52 @@
       <c r="K12" s="28">
         <v>22288</v>
       </c>
-      <c r="L12" s="83">
+      <c r="L12" s="27"/>
+      <c r="M12" s="79">
         <f t="shared" si="3"/>
         <v>1.0329511414110113E-4</v>
       </c>
-      <c r="M12" s="15" t="s">
+      <c r="N12" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="N12" s="4">
+      <c r="O12" s="4">
         <v>1</v>
       </c>
-      <c r="O12" s="66">
+      <c r="P12" s="75">
+        <v>10</v>
+      </c>
+      <c r="Q12" s="66">
         <f>1000*(C11+C12)</f>
         <v>40970000</v>
       </c>
-      <c r="P12" s="67">
+      <c r="R12" s="67">
         <f t="shared" si="4"/>
         <v>2.4408103490358799E-2</v>
       </c>
-      <c r="Q12" s="69">
+      <c r="S12" s="69">
         <f t="shared" si="0"/>
         <v>0.40605309368866854</v>
       </c>
-      <c r="R12" s="69">
+      <c r="T12" s="69">
         <f t="shared" si="0"/>
         <v>0.59394690631133151</v>
       </c>
-      <c r="S12" s="71">
+      <c r="U12" s="71">
         <v>20.041</v>
       </c>
-      <c r="T12" s="71">
+      <c r="V12" s="71">
         <v>20.928999999999998</v>
       </c>
-      <c r="U12" s="75">
-        <v>10</v>
-      </c>
-      <c r="V12" s="73">
+      <c r="W12" s="73">
         <f t="shared" si="1"/>
         <v>2.0261119389684574E-2</v>
       </c>
-      <c r="W12" s="73">
+      <c r="X12" s="73">
         <f t="shared" si="2"/>
         <v>2.8379134517240744E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="19" t="s">
         <v>122</v>
       </c>
@@ -6308,51 +7307,52 @@
       <c r="K13" s="28">
         <v>22527</v>
       </c>
-      <c r="L13" s="83">
+      <c r="L13" s="27"/>
+      <c r="M13" s="79">
         <f t="shared" si="3"/>
         <v>9.2965602726991013E-4</v>
       </c>
-      <c r="M13" s="15" t="s">
+      <c r="N13" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="N13" s="4">
+      <c r="O13" s="4">
         <v>9</v>
       </c>
-      <c r="O13" s="66">
+      <c r="P13" s="75">
+        <v>20</v>
+      </c>
+      <c r="Q13" s="66">
         <f>1000*(C13+C14)</f>
         <v>42937000</v>
       </c>
-      <c r="P13" s="67">
+      <c r="R13" s="67">
         <f t="shared" si="4"/>
         <v>0.20960942776626221</v>
       </c>
-      <c r="Q13" s="69">
+      <c r="S13" s="69">
         <f t="shared" si="0"/>
         <v>3.6544778431980167</v>
       </c>
-      <c r="R13" s="69">
+      <c r="T13" s="69">
         <f t="shared" si="0"/>
         <v>5.3455221568019837</v>
       </c>
-      <c r="S13" s="71">
+      <c r="U13" s="71">
         <v>21.007000000000001</v>
       </c>
-      <c r="T13" s="71">
+      <c r="V13" s="71">
         <v>21.931000000000001</v>
       </c>
-      <c r="U13" s="75">
-        <v>20</v>
-      </c>
-      <c r="V13" s="73">
+      <c r="W13" s="73">
         <f t="shared" si="1"/>
         <v>0.17396476618260659</v>
       </c>
-      <c r="W13" s="73">
+      <c r="X13" s="73">
         <f t="shared" si="2"/>
         <v>0.24374274573899884</v>
       </c>
     </row>
-    <row r="14" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="19" t="s">
         <v>121</v>
       </c>
@@ -6386,51 +7386,52 @@
       <c r="K14" s="28">
         <v>23384</v>
       </c>
-      <c r="L14" s="83">
+      <c r="L14" s="27"/>
+      <c r="M14" s="79">
         <f t="shared" si="3"/>
         <v>9.2965602726991017E-3</v>
       </c>
-      <c r="M14" s="15" t="s">
+      <c r="N14" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="N14" s="4">
+      <c r="O14" s="4">
         <v>90</v>
       </c>
-      <c r="O14" s="66">
+      <c r="P14" s="75">
+        <v>30</v>
+      </c>
+      <c r="Q14" s="66">
         <f>1000*(C15+C16)</f>
         <v>46491000</v>
       </c>
-      <c r="P14" s="67">
+      <c r="R14" s="67">
         <f t="shared" si="4"/>
         <v>1.9358585532683745</v>
       </c>
-      <c r="Q14" s="69">
+      <c r="S14" s="69">
         <f t="shared" si="0"/>
         <v>36.54477843198017</v>
       </c>
-      <c r="R14" s="69">
+      <c r="T14" s="69">
         <f t="shared" si="0"/>
         <v>53.455221568019837</v>
       </c>
-      <c r="S14" s="71">
+      <c r="U14" s="71">
         <v>22.812999999999999</v>
       </c>
-      <c r="T14" s="71">
+      <c r="V14" s="71">
         <v>23.678000000000001</v>
       </c>
-      <c r="U14" s="75">
-        <v>30</v>
-      </c>
-      <c r="V14" s="73">
+      <c r="W14" s="73">
         <f t="shared" si="1"/>
         <v>1.6019277794231435</v>
       </c>
-      <c r="W14" s="73">
+      <c r="X14" s="73">
         <f t="shared" si="2"/>
         <v>2.2575902343111678</v>
       </c>
     </row>
-    <row r="15" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="19" t="s">
         <v>120</v>
       </c>
@@ -6464,51 +7465,52 @@
       <c r="K15" s="28">
         <v>24387</v>
       </c>
-      <c r="L15" s="83">
+      <c r="L15" s="27"/>
+      <c r="M15" s="79">
         <f t="shared" si="3"/>
         <v>2.2415039768618944E-2</v>
       </c>
-      <c r="M15" s="15" t="s">
+      <c r="N15" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="N15" s="4">
+      <c r="O15" s="4">
         <v>217</v>
       </c>
-      <c r="O15" s="66">
+      <c r="P15" s="75">
+        <v>40</v>
+      </c>
+      <c r="Q15" s="66">
         <f>1000*(C17+C18)</f>
         <v>42352000</v>
       </c>
-      <c r="P15" s="67">
+      <c r="R15" s="67">
         <f t="shared" si="4"/>
         <v>5.1237249716660367</v>
       </c>
-      <c r="Q15" s="69">
+      <c r="S15" s="69">
         <f t="shared" si="0"/>
         <v>88.113521330441074</v>
       </c>
-      <c r="R15" s="69">
+      <c r="T15" s="69">
         <f t="shared" si="0"/>
         <v>128.88647866955893</v>
       </c>
-      <c r="S15" s="71">
+      <c r="U15" s="71">
         <v>21.193999999999999</v>
       </c>
-      <c r="T15" s="71">
+      <c r="V15" s="71">
         <v>21.158000000000001</v>
       </c>
-      <c r="U15" s="75">
-        <v>40</v>
-      </c>
-      <c r="V15" s="73">
+      <c r="W15" s="73">
         <f t="shared" si="1"/>
         <v>4.1574748197811209</v>
       </c>
-      <c r="W15" s="73">
+      <c r="X15" s="73">
         <f t="shared" si="2"/>
         <v>6.0916191827941635</v>
       </c>
     </row>
-    <row r="16" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="19" t="s">
         <v>119</v>
       </c>
@@ -6542,51 +7544,52 @@
       <c r="K16" s="28">
         <v>25155</v>
       </c>
-      <c r="L16" s="83">
+      <c r="L16" s="27"/>
+      <c r="M16" s="79">
         <f t="shared" si="3"/>
         <v>5.7638673690734429E-2</v>
       </c>
-      <c r="M16" s="15" t="s">
+      <c r="N16" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="N16" s="4">
+      <c r="O16" s="4">
         <v>558</v>
       </c>
-      <c r="O16" s="66">
+      <c r="P16" s="75">
+        <v>50</v>
+      </c>
+      <c r="Q16" s="66">
         <f>1000*(C19+C20)</f>
         <v>40615000</v>
       </c>
-      <c r="P16" s="67">
+      <c r="R16" s="67">
         <f t="shared" si="4"/>
         <v>13.738766465591532</v>
       </c>
-      <c r="Q16" s="69">
+      <c r="S16" s="69">
         <f t="shared" si="0"/>
         <v>226.57762627827705</v>
       </c>
-      <c r="R16" s="69">
+      <c r="T16" s="69">
         <f t="shared" si="0"/>
         <v>331.42237372172298</v>
       </c>
-      <c r="S16" s="71">
+      <c r="U16" s="71">
         <v>20.558</v>
       </c>
-      <c r="T16" s="71">
+      <c r="V16" s="71">
         <v>20.056999999999999</v>
       </c>
-      <c r="U16" s="75">
-        <v>50</v>
-      </c>
-      <c r="V16" s="73">
+      <c r="W16" s="73">
         <f t="shared" si="1"/>
         <v>11.021384681305431</v>
       </c>
-      <c r="W16" s="73">
+      <c r="X16" s="73">
         <f t="shared" si="2"/>
         <v>16.524025214225606</v>
       </c>
     </row>
-    <row r="17" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="19" t="s">
         <v>118</v>
       </c>
@@ -6620,51 +7623,52 @@
       <c r="K17" s="28">
         <v>25470</v>
       </c>
-      <c r="L17" s="83">
+      <c r="L17" s="27"/>
+      <c r="M17" s="79">
         <f t="shared" si="3"/>
         <v>0.13128809007333953</v>
       </c>
-      <c r="M17" s="15" t="s">
+      <c r="N17" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="N17" s="3">
+      <c r="O17" s="3">
         <v>1271</v>
       </c>
-      <c r="O17" s="66">
+      <c r="P17" s="75">
+        <v>60</v>
+      </c>
+      <c r="Q17" s="66">
         <f>1000*(C21+C22)</f>
         <v>42783000</v>
       </c>
-      <c r="P17" s="67">
+      <c r="R17" s="67">
         <f t="shared" si="4"/>
         <v>29.708061613257602</v>
       </c>
-      <c r="Q17" s="69">
+      <c r="S17" s="69">
         <f t="shared" si="0"/>
         <v>516.09348207829771</v>
       </c>
-      <c r="R17" s="69">
+      <c r="T17" s="69">
         <f t="shared" si="0"/>
         <v>754.9065179217024</v>
       </c>
-      <c r="S17" s="71">
+      <c r="U17" s="71">
         <v>22.091999999999999</v>
       </c>
-      <c r="T17" s="71">
+      <c r="V17" s="71">
         <v>20.690999999999999</v>
       </c>
-      <c r="U17" s="75">
-        <v>60</v>
-      </c>
-      <c r="V17" s="73">
+      <c r="W17" s="73">
         <f t="shared" si="1"/>
         <v>23.361102755671634</v>
       </c>
-      <c r="W17" s="73">
+      <c r="X17" s="73">
         <f t="shared" si="2"/>
         <v>36.484776855719993</v>
       </c>
     </row>
-    <row r="18" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="19" t="s">
         <v>117</v>
       </c>
@@ -6698,51 +7702,52 @@
       <c r="K18" s="28">
         <v>25218</v>
       </c>
-      <c r="L18" s="83">
+      <c r="L18" s="27"/>
+      <c r="M18" s="79">
         <f t="shared" si="3"/>
         <v>0.22229108563164962</v>
       </c>
-      <c r="M18" s="15" t="s">
+      <c r="N18" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="N18" s="3">
+      <c r="O18" s="3">
         <v>2152</v>
       </c>
-      <c r="O18" s="66">
+      <c r="P18" s="75">
+        <v>70</v>
+      </c>
+      <c r="Q18" s="66">
         <f>1000*(C23+C24)</f>
         <v>32789000</v>
       </c>
-      <c r="P18" s="67">
+      <c r="R18" s="67">
         <f t="shared" si="4"/>
         <v>65.631766751044552</v>
       </c>
-      <c r="Q18" s="69">
+      <c r="S18" s="69">
         <f t="shared" si="0"/>
         <v>873.82625761801467</v>
       </c>
-      <c r="R18" s="69">
+      <c r="T18" s="69">
         <f t="shared" si="0"/>
         <v>1278.1737423819854</v>
       </c>
-      <c r="S18" s="71">
+      <c r="U18" s="71">
         <v>17.46</v>
       </c>
-      <c r="T18" s="71">
+      <c r="V18" s="71">
         <v>15.329000000000001</v>
       </c>
-      <c r="U18" s="75">
-        <v>70</v>
-      </c>
-      <c r="V18" s="73">
+      <c r="W18" s="73">
         <f t="shared" si="1"/>
         <v>50.047322887629704</v>
       </c>
-      <c r="W18" s="73">
+      <c r="X18" s="73">
         <f t="shared" si="2"/>
         <v>83.382721794114772</v>
       </c>
     </row>
-    <row r="19" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="19" t="s">
         <v>116</v>
       </c>
@@ -6776,51 +7781,52 @@
       <c r="K19" s="28">
         <v>24680</v>
       </c>
-      <c r="L19" s="83">
+      <c r="L19" s="27"/>
+      <c r="M19" s="79">
         <f t="shared" si="3"/>
         <v>0.27114967462039047</v>
       </c>
-      <c r="M19" s="15" t="s">
+      <c r="N19" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="N19" s="3">
+      <c r="O19" s="3">
         <v>2625</v>
       </c>
-      <c r="O19" s="66">
+      <c r="P19" s="75">
+        <v>80</v>
+      </c>
+      <c r="Q19" s="66">
         <f>1000*(C25+C26)</f>
         <v>16561000</v>
       </c>
-      <c r="P19" s="67">
+      <c r="R19" s="67">
         <f t="shared" si="4"/>
         <v>158.50492120041062</v>
       </c>
-      <c r="Q19" s="69">
+      <c r="S19" s="69">
         <f t="shared" si="0"/>
         <v>1065.8893709327549</v>
       </c>
-      <c r="R19" s="69">
+      <c r="T19" s="69">
         <f t="shared" si="0"/>
         <v>1559.1106290672453</v>
       </c>
-      <c r="S19" s="71">
+      <c r="U19" s="71">
         <v>9.2940000000000005</v>
       </c>
-      <c r="T19" s="71">
+      <c r="V19" s="71">
         <v>7.2670000000000003</v>
       </c>
-      <c r="U19" s="75">
-        <v>80</v>
-      </c>
-      <c r="V19" s="73">
+      <c r="W19" s="73">
         <f t="shared" si="1"/>
         <v>114.6857511225258</v>
       </c>
-      <c r="W19" s="73">
+      <c r="X19" s="73">
         <f t="shared" si="2"/>
         <v>214.54666699700635</v>
       </c>
     </row>
-    <row r="20" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="19" t="s">
         <v>115</v>
       </c>
@@ -6854,51 +7860,52 @@
       <c r="K20" s="28">
         <v>24681</v>
       </c>
-      <c r="L20" s="83">
+      <c r="L20" s="27"/>
+      <c r="M20" s="79">
         <f t="shared" si="3"/>
         <v>0.2846813345728747</v>
       </c>
-      <c r="M20" s="15" t="s">
+      <c r="N20" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="N20" s="3">
+      <c r="O20" s="3">
         <v>2756</v>
       </c>
-      <c r="O20" s="66">
+      <c r="P20" s="75">
+        <v>90</v>
+      </c>
+      <c r="Q20" s="66">
         <f>1000*(C27+C28+C29+C30)</f>
         <v>6701000</v>
       </c>
-      <c r="P20" s="67">
+      <c r="R20" s="67">
         <f t="shared" si="4"/>
         <v>411.28189822414566</v>
       </c>
-      <c r="Q20" s="69">
+      <c r="S20" s="69">
         <f t="shared" si="0"/>
         <v>1119.0823262059705</v>
       </c>
-      <c r="R20" s="69">
+      <c r="T20" s="69">
         <f t="shared" si="0"/>
         <v>1636.9176737940297</v>
       </c>
-      <c r="S20" s="71">
+      <c r="U20" s="71">
         <v>4.2830000000000004</v>
       </c>
-      <c r="T20" s="71">
+      <c r="V20" s="71">
         <v>2.4180000000000001</v>
       </c>
-      <c r="U20" s="75">
-        <v>90</v>
-      </c>
-      <c r="V20" s="73">
+      <c r="W20" s="73">
         <f t="shared" si="1"/>
         <v>261.28468975156909</v>
       </c>
-      <c r="W20" s="73">
+      <c r="X20" s="73">
         <f t="shared" si="2"/>
         <v>676.97174267743162</v>
       </c>
     </row>
-    <row r="21" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="19" t="s">
         <v>114</v>
       </c>
@@ -6932,16 +7939,17 @@
       <c r="K21" s="28">
         <v>24087</v>
       </c>
-      <c r="L21" s="15"/>
+      <c r="L21" s="27"/>
       <c r="M21" s="15"/>
-      <c r="N21" s="76">
-        <f>+S7+T7</f>
+      <c r="N21" s="15"/>
+      <c r="O21" s="76">
+        <f>+U7+V7</f>
         <v>9681</v>
       </c>
-      <c r="O21" s="15"/>
-      <c r="P21" s="15"/>
-    </row>
-    <row r="22" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="Q21" s="15"/>
+      <c r="R21" s="15"/>
+    </row>
+    <row r="22" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="19" t="s">
         <v>113</v>
       </c>
@@ -6975,13 +7983,14 @@
       <c r="K22" s="28">
         <v>23525</v>
       </c>
-      <c r="L22" s="15"/>
+      <c r="L22" s="27"/>
       <c r="M22" s="15"/>
       <c r="N22" s="15"/>
       <c r="O22" s="15"/>
-      <c r="P22" s="15"/>
-    </row>
-    <row r="23" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="Q22" s="15"/>
+      <c r="R22" s="15"/>
+    </row>
+    <row r="23" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="19" t="s">
         <v>112</v>
       </c>
@@ -7015,13 +8024,14 @@
       <c r="K23" s="28">
         <v>23269</v>
       </c>
-      <c r="L23" s="15"/>
+      <c r="L23" s="27"/>
       <c r="M23" s="15"/>
       <c r="N23" s="15"/>
       <c r="O23" s="15"/>
-      <c r="P23" s="15"/>
-    </row>
-    <row r="24" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="Q23" s="15"/>
+      <c r="R23" s="15"/>
+    </row>
+    <row r="24" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="19" t="s">
         <v>111</v>
       </c>
@@ -7055,13 +8065,14 @@
       <c r="K24" s="28">
         <v>20884</v>
       </c>
-      <c r="L24" s="15"/>
+      <c r="L24" s="27"/>
       <c r="M24" s="15"/>
       <c r="N24" s="15"/>
       <c r="O24" s="15"/>
-      <c r="P24" s="15"/>
-    </row>
-    <row r="25" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="Q24" s="15"/>
+      <c r="R24" s="15"/>
+    </row>
+    <row r="25" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="19" t="s">
         <v>110</v>
       </c>
@@ -7095,13 +8106,14 @@
       <c r="K25" s="28">
         <v>17725</v>
       </c>
-      <c r="L25" s="15"/>
+      <c r="L25" s="27"/>
       <c r="M25" s="15"/>
       <c r="N25" s="15"/>
       <c r="O25" s="15"/>
-      <c r="P25" s="15"/>
-    </row>
-    <row r="26" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="Q25" s="15"/>
+      <c r="R25" s="15"/>
+    </row>
+    <row r="26" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="19" t="s">
         <v>109</v>
       </c>
@@ -7135,13 +8147,14 @@
       <c r="K26" s="28">
         <v>13779</v>
       </c>
-      <c r="L26" s="15"/>
+      <c r="L26" s="27"/>
       <c r="M26" s="15"/>
       <c r="N26" s="15"/>
       <c r="O26" s="15"/>
-      <c r="P26" s="15"/>
-    </row>
-    <row r="27" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="Q26" s="15"/>
+      <c r="R26" s="15"/>
+    </row>
+    <row r="27" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="19" t="s">
         <v>108</v>
       </c>
@@ -7175,13 +8188,14 @@
       <c r="K27" s="28">
         <v>9808</v>
       </c>
-      <c r="L27" s="15"/>
+      <c r="L27" s="27"/>
       <c r="M27" s="15"/>
       <c r="N27" s="15"/>
       <c r="O27" s="15"/>
-      <c r="P27" s="15"/>
-    </row>
-    <row r="28" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="Q27" s="15"/>
+      <c r="R27" s="15"/>
+    </row>
+    <row r="28" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="19" t="s">
         <v>107</v>
       </c>
@@ -7215,13 +8229,14 @@
       <c r="K28" s="28">
         <v>5957</v>
       </c>
-      <c r="L28" s="15"/>
+      <c r="L28" s="27"/>
       <c r="M28" s="15"/>
       <c r="N28" s="15"/>
       <c r="O28" s="15"/>
-      <c r="P28" s="15"/>
-    </row>
-    <row r="29" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="Q28" s="15"/>
+      <c r="R28" s="15"/>
+    </row>
+    <row r="29" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="19" t="s">
         <v>106</v>
       </c>
@@ -7255,13 +8270,14 @@
       <c r="K29" s="28">
         <v>2666</v>
       </c>
-      <c r="L29" s="15"/>
+      <c r="L29" s="27"/>
       <c r="M29" s="15"/>
       <c r="N29" s="15"/>
       <c r="O29" s="15"/>
-      <c r="P29" s="15"/>
-    </row>
-    <row r="30" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="Q29" s="15"/>
+      <c r="R29" s="15"/>
+    </row>
+    <row r="30" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="19" t="s">
         <v>105</v>
       </c>
@@ -7295,13 +8311,14 @@
       <c r="K30" s="28">
         <v>589</v>
       </c>
-      <c r="L30" s="15"/>
+      <c r="L30" s="27"/>
       <c r="M30" s="15"/>
       <c r="N30" s="15"/>
       <c r="O30" s="15"/>
-      <c r="P30" s="15"/>
-    </row>
-    <row r="31" spans="1:29" s="37" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="Q30" s="15"/>
+      <c r="R30" s="15"/>
+    </row>
+    <row r="31" spans="1:30" s="37" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="34" t="s">
         <v>128</v>
       </c>
@@ -7335,13 +8352,13 @@
       <c r="K31" s="36">
         <v>200871</v>
       </c>
-      <c r="L31" s="15"/>
+      <c r="L31" s="27"/>
       <c r="M31" s="15"/>
       <c r="N31" s="15"/>
       <c r="O31" s="15"/>
-      <c r="P31" s="15"/>
-      <c r="Q31" s="54"/>
-      <c r="R31" s="54"/>
+      <c r="P31" s="54"/>
+      <c r="Q31" s="15"/>
+      <c r="R31" s="15"/>
       <c r="S31" s="54"/>
       <c r="T31" s="54"/>
       <c r="U31" s="54"/>
@@ -7353,8 +8370,9 @@
       <c r="AA31" s="54"/>
       <c r="AB31" s="54"/>
       <c r="AC31" s="54"/>
-    </row>
-    <row r="32" spans="1:29" s="52" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AD31" s="54"/>
+    </row>
+    <row r="32" spans="1:30" s="52" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="53" t="s">
         <v>126</v>
       </c>
@@ -7388,13 +8406,13 @@
       <c r="K32" s="50">
         <v>41.86</v>
       </c>
-      <c r="L32" s="51"/>
+      <c r="L32" s="49"/>
       <c r="M32" s="51"/>
       <c r="N32" s="51"/>
       <c r="O32" s="51"/>
-      <c r="P32" s="51"/>
-      <c r="Q32" s="54"/>
-      <c r="R32" s="54"/>
+      <c r="P32" s="54"/>
+      <c r="Q32" s="51"/>
+      <c r="R32" s="51"/>
       <c r="S32" s="54"/>
       <c r="T32" s="54"/>
       <c r="U32" s="54"/>
@@ -7406,8 +8424,9 @@
       <c r="AA32" s="54"/>
       <c r="AB32" s="54"/>
       <c r="AC32" s="54"/>
-    </row>
-    <row r="33" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AD32" s="54"/>
+    </row>
+    <row r="33" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="38"/>
       <c r="B33" s="58"/>
       <c r="C33" s="40"/>
@@ -7419,13 +8438,14 @@
       <c r="I33" s="40"/>
       <c r="J33" s="40"/>
       <c r="K33" s="41"/>
-      <c r="L33" s="15"/>
+      <c r="L33" s="40"/>
       <c r="M33" s="15"/>
       <c r="N33" s="15"/>
       <c r="O33" s="15"/>
-      <c r="P33" s="15"/>
-    </row>
-    <row r="34" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="Q33" s="15"/>
+      <c r="R33" s="15"/>
+    </row>
+    <row r="34" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="39" t="s">
         <v>125</v>
       </c>
@@ -7459,16 +8479,15 @@
       <c r="K34" s="28">
         <v>11310</v>
       </c>
-      <c r="L34" s="15"/>
-      <c r="M34" s="15"/>
-      <c r="N34" s="15"/>
-      <c r="O34" s="15">
+      <c r="L34" s="15">
         <f>C34/5</f>
         <v>2089.1999999999998</v>
       </c>
-      <c r="P34" s="15"/>
-    </row>
-    <row r="35" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="N34" s="15"/>
+      <c r="O34" s="15"/>
+      <c r="R34" s="15"/>
+    </row>
+    <row r="35" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="39" t="s">
         <v>124</v>
       </c>
@@ -7502,16 +8521,15 @@
       <c r="K35" s="28">
         <v>11364</v>
       </c>
-      <c r="L35" s="15"/>
-      <c r="M35" s="15"/>
+      <c r="L35" s="1">
+        <f>C34-L34</f>
+        <v>8356.7999999999993</v>
+      </c>
       <c r="N35" s="15"/>
-      <c r="O35" s="1">
-        <f>C34-O34</f>
-        <v>8356.7999999999993</v>
-      </c>
-      <c r="P35" s="15"/>
-    </row>
-    <row r="36" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="O35" s="15"/>
+      <c r="R35" s="15"/>
+    </row>
+    <row r="36" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="39" t="s">
         <v>123</v>
       </c>
@@ -7545,16 +8563,15 @@
       <c r="K36" s="28">
         <v>11380</v>
       </c>
-      <c r="L36" s="15"/>
-      <c r="M36" s="15"/>
-      <c r="N36" s="15"/>
-      <c r="O36" s="1">
+      <c r="L36" s="1">
         <f>+C35+C36</f>
         <v>20929</v>
       </c>
-      <c r="P36" s="15"/>
-    </row>
-    <row r="37" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="N36" s="15"/>
+      <c r="O36" s="15"/>
+      <c r="R36" s="15"/>
+    </row>
+    <row r="37" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="39" t="s">
         <v>122</v>
       </c>
@@ -7588,16 +8605,15 @@
       <c r="K37" s="28">
         <v>11501</v>
       </c>
-      <c r="L37" s="15"/>
-      <c r="M37" s="15"/>
-      <c r="N37" s="15"/>
-      <c r="O37" s="1">
+      <c r="L37" s="1">
         <f>+C37+C38</f>
         <v>21931</v>
       </c>
-      <c r="P37" s="15"/>
-    </row>
-    <row r="38" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="N37" s="15"/>
+      <c r="O37" s="15"/>
+      <c r="R37" s="15"/>
+    </row>
+    <row r="38" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="39" t="s">
         <v>121</v>
       </c>
@@ -7631,16 +8647,15 @@
       <c r="K38" s="28">
         <v>11931</v>
       </c>
-      <c r="L38" s="15"/>
-      <c r="M38" s="15"/>
-      <c r="N38" s="15"/>
-      <c r="O38" s="1">
+      <c r="L38" s="1">
         <f>+C39+C40</f>
         <v>23678</v>
       </c>
-      <c r="P38" s="15"/>
-    </row>
-    <row r="39" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="N38" s="15"/>
+      <c r="O38" s="15"/>
+      <c r="R38" s="15"/>
+    </row>
+    <row r="39" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="39" t="s">
         <v>120</v>
       </c>
@@ -7674,16 +8689,15 @@
       <c r="K39" s="28">
         <v>12412</v>
       </c>
-      <c r="L39" s="15"/>
-      <c r="M39" s="15"/>
-      <c r="N39" s="15"/>
-      <c r="O39" s="1">
+      <c r="L39" s="1">
         <f>+C41+C42</f>
         <v>21158</v>
       </c>
-      <c r="P39" s="15"/>
-    </row>
-    <row r="40" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="N39" s="15"/>
+      <c r="O39" s="15"/>
+      <c r="R39" s="15"/>
+    </row>
+    <row r="40" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="39" t="s">
         <v>119</v>
       </c>
@@ -7717,16 +8731,15 @@
       <c r="K40" s="28">
         <v>12797</v>
       </c>
-      <c r="L40" s="15"/>
-      <c r="M40" s="15"/>
-      <c r="N40" s="15"/>
-      <c r="O40" s="1">
+      <c r="L40" s="1">
         <f>+C43+C44</f>
         <v>20057</v>
       </c>
-      <c r="P40" s="15"/>
-    </row>
-    <row r="41" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="N40" s="15"/>
+      <c r="O40" s="15"/>
+      <c r="R40" s="15"/>
+    </row>
+    <row r="41" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="39" t="s">
         <v>118</v>
       </c>
@@ -7760,16 +8773,15 @@
       <c r="K41" s="28">
         <v>12948</v>
       </c>
-      <c r="L41" s="15"/>
-      <c r="M41" s="15"/>
-      <c r="N41" s="15"/>
-      <c r="O41" s="1">
+      <c r="L41" s="1">
         <f>+C45+C46</f>
         <v>20691</v>
       </c>
-      <c r="P41" s="15"/>
-    </row>
-    <row r="42" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="N41" s="15"/>
+      <c r="O41" s="15"/>
+      <c r="R41" s="15"/>
+    </row>
+    <row r="42" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" s="39" t="s">
         <v>117</v>
       </c>
@@ -7803,16 +8815,15 @@
       <c r="K42" s="28">
         <v>12795</v>
       </c>
-      <c r="L42" s="15"/>
-      <c r="M42" s="15"/>
-      <c r="N42" s="15"/>
-      <c r="O42" s="1">
+      <c r="L42" s="1">
         <f>+C47+C48</f>
         <v>15329</v>
       </c>
-      <c r="P42" s="15"/>
-    </row>
-    <row r="43" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="N42" s="15"/>
+      <c r="O42" s="15"/>
+      <c r="R42" s="15"/>
+    </row>
+    <row r="43" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43" s="39" t="s">
         <v>116</v>
       </c>
@@ -7846,16 +8857,15 @@
       <c r="K43" s="28">
         <v>12505</v>
       </c>
-      <c r="L43" s="15"/>
-      <c r="M43" s="15"/>
-      <c r="N43" s="15"/>
-      <c r="O43" s="1">
+      <c r="L43" s="1">
         <f>+C49+C50</f>
         <v>7267</v>
       </c>
-      <c r="P43" s="15"/>
-    </row>
-    <row r="44" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="N43" s="15"/>
+      <c r="O43" s="15"/>
+      <c r="R43" s="15"/>
+    </row>
+    <row r="44" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A44" s="39" t="s">
         <v>115</v>
       </c>
@@ -7889,16 +8899,15 @@
       <c r="K44" s="28">
         <v>12447</v>
       </c>
-      <c r="L44" s="15"/>
-      <c r="M44" s="15"/>
-      <c r="N44" s="15"/>
-      <c r="O44" s="1">
+      <c r="L44" s="1">
         <f>+C51+C52+C53+C54</f>
         <v>2418</v>
       </c>
-      <c r="P44" s="15"/>
-    </row>
-    <row r="45" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="N44" s="15"/>
+      <c r="O44" s="15"/>
+      <c r="R44" s="15"/>
+    </row>
+    <row r="45" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A45" s="39" t="s">
         <v>114</v>
       </c>
@@ -7932,13 +8941,14 @@
       <c r="K45" s="28">
         <v>12076</v>
       </c>
-      <c r="L45" s="15"/>
+      <c r="L45" s="27"/>
       <c r="M45" s="15"/>
       <c r="N45" s="15"/>
       <c r="O45" s="15"/>
-      <c r="P45" s="15"/>
-    </row>
-    <row r="46" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="Q45" s="15"/>
+      <c r="R45" s="15"/>
+    </row>
+    <row r="46" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A46" s="39" t="s">
         <v>113</v>
       </c>
@@ -7972,13 +8982,14 @@
       <c r="K46" s="28">
         <v>11742</v>
       </c>
-      <c r="L46" s="15"/>
+      <c r="L46" s="27"/>
       <c r="M46" s="15"/>
       <c r="N46" s="15"/>
       <c r="O46" s="15"/>
-      <c r="P46" s="15"/>
-    </row>
-    <row r="47" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="Q46" s="15"/>
+      <c r="R46" s="15"/>
+    </row>
+    <row r="47" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A47" s="39" t="s">
         <v>112</v>
       </c>
@@ -8012,13 +9023,14 @@
       <c r="K47" s="28">
         <v>11542</v>
       </c>
-      <c r="L47" s="15"/>
+      <c r="L47" s="27"/>
       <c r="M47" s="15"/>
       <c r="N47" s="15"/>
       <c r="O47" s="15"/>
-      <c r="P47" s="15"/>
-    </row>
-    <row r="48" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="Q47" s="15"/>
+      <c r="R47" s="15"/>
+    </row>
+    <row r="48" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A48" s="39" t="s">
         <v>111</v>
       </c>
@@ -8052,13 +9064,14 @@
       <c r="K48" s="28">
         <v>10128</v>
       </c>
-      <c r="L48" s="15"/>
+      <c r="L48" s="27"/>
       <c r="M48" s="15"/>
       <c r="N48" s="15"/>
       <c r="O48" s="15"/>
-      <c r="P48" s="15"/>
-    </row>
-    <row r="49" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="Q48" s="15"/>
+      <c r="R48" s="15"/>
+    </row>
+    <row r="49" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A49" s="39" t="s">
         <v>110</v>
       </c>
@@ -8092,13 +9105,14 @@
       <c r="K49" s="28">
         <v>8315</v>
       </c>
-      <c r="L49" s="15"/>
+      <c r="L49" s="27"/>
       <c r="M49" s="15"/>
       <c r="N49" s="15"/>
       <c r="O49" s="15"/>
-      <c r="P49" s="15"/>
-    </row>
-    <row r="50" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="Q49" s="15"/>
+      <c r="R49" s="15"/>
+    </row>
+    <row r="50" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A50" s="39" t="s">
         <v>109</v>
       </c>
@@ -8132,13 +9146,14 @@
       <c r="K50" s="28">
         <v>6202</v>
       </c>
-      <c r="L50" s="15"/>
+      <c r="L50" s="27"/>
       <c r="M50" s="15"/>
       <c r="N50" s="15"/>
       <c r="O50" s="15"/>
-      <c r="P50" s="15"/>
-    </row>
-    <row r="51" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="Q50" s="15"/>
+      <c r="R50" s="15"/>
+    </row>
+    <row r="51" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A51" s="39" t="s">
         <v>108</v>
       </c>
@@ -8172,13 +9187,14 @@
       <c r="K51" s="28">
         <v>4127</v>
       </c>
-      <c r="L51" s="15"/>
+      <c r="L51" s="27"/>
       <c r="M51" s="15"/>
       <c r="N51" s="15"/>
       <c r="O51" s="15"/>
-      <c r="P51" s="15"/>
-    </row>
-    <row r="52" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="Q51" s="15"/>
+      <c r="R51" s="15"/>
+    </row>
+    <row r="52" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A52" s="39" t="s">
         <v>107</v>
       </c>
@@ -8212,13 +9228,14 @@
       <c r="K52" s="28">
         <v>2289</v>
       </c>
-      <c r="L52" s="15"/>
+      <c r="L52" s="27"/>
       <c r="M52" s="15"/>
       <c r="N52" s="15"/>
       <c r="O52" s="15"/>
-      <c r="P52" s="15"/>
-    </row>
-    <row r="53" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="Q52" s="15"/>
+      <c r="R52" s="15"/>
+    </row>
+    <row r="53" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A53" s="39" t="s">
         <v>106</v>
       </c>
@@ -8252,13 +9269,14 @@
       <c r="K53" s="28">
         <v>893</v>
       </c>
-      <c r="L53" s="15"/>
+      <c r="L53" s="27"/>
       <c r="M53" s="15"/>
       <c r="N53" s="15"/>
       <c r="O53" s="15"/>
-      <c r="P53" s="15"/>
-    </row>
-    <row r="54" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="Q53" s="15"/>
+      <c r="R53" s="15"/>
+    </row>
+    <row r="54" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A54" s="39" t="s">
         <v>105</v>
       </c>
@@ -8292,13 +9310,14 @@
       <c r="K54" s="28">
         <v>168</v>
       </c>
-      <c r="L54" s="15"/>
+      <c r="L54" s="27"/>
       <c r="M54" s="15"/>
       <c r="N54" s="15"/>
       <c r="O54" s="15"/>
-      <c r="P54" s="15"/>
-    </row>
-    <row r="55" spans="1:29" s="37" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="Q54" s="15"/>
+      <c r="R54" s="15"/>
+    </row>
+    <row r="55" spans="1:30" s="37" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A55" s="33" t="s">
         <v>127</v>
       </c>
@@ -8332,13 +9351,13 @@
       <c r="K55" s="36">
         <v>203612</v>
       </c>
-      <c r="L55" s="15"/>
+      <c r="L55" s="27"/>
       <c r="M55" s="15"/>
       <c r="N55" s="15"/>
       <c r="O55" s="15"/>
-      <c r="P55" s="15"/>
-      <c r="Q55" s="54"/>
-      <c r="R55" s="54"/>
+      <c r="P55" s="54"/>
+      <c r="Q55" s="15"/>
+      <c r="R55" s="15"/>
       <c r="S55" s="54"/>
       <c r="T55" s="54"/>
       <c r="U55" s="54"/>
@@ -8350,8 +9369,9 @@
       <c r="AA55" s="54"/>
       <c r="AB55" s="54"/>
       <c r="AC55" s="54"/>
-    </row>
-    <row r="56" spans="1:29" s="52" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AD55" s="54"/>
+    </row>
+    <row r="56" spans="1:30" s="52" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A56" s="53" t="s">
         <v>126</v>
       </c>
@@ -8385,13 +9405,13 @@
       <c r="K56" s="50">
         <v>43.94</v>
       </c>
-      <c r="L56" s="51"/>
+      <c r="L56" s="49"/>
       <c r="M56" s="51"/>
       <c r="N56" s="51"/>
       <c r="O56" s="51"/>
-      <c r="P56" s="51"/>
-      <c r="Q56" s="54"/>
-      <c r="R56" s="54"/>
+      <c r="P56" s="54"/>
+      <c r="Q56" s="51"/>
+      <c r="R56" s="51"/>
       <c r="S56" s="54"/>
       <c r="T56" s="54"/>
       <c r="U56" s="54"/>
@@ -8403,8 +9423,9 @@
       <c r="AA56" s="54"/>
       <c r="AB56" s="54"/>
       <c r="AC56" s="54"/>
-    </row>
-    <row r="57" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AD56" s="54"/>
+    </row>
+    <row r="57" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A57" s="38"/>
       <c r="B57" s="58"/>
       <c r="C57" s="40"/>
@@ -8416,13 +9437,14 @@
       <c r="I57" s="40"/>
       <c r="J57" s="40"/>
       <c r="K57" s="41"/>
-      <c r="L57" s="15"/>
+      <c r="L57" s="40"/>
       <c r="M57" s="15"/>
       <c r="N57" s="15"/>
       <c r="O57" s="15"/>
-      <c r="P57" s="15"/>
-    </row>
-    <row r="58" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="Q57" s="15"/>
+      <c r="R57" s="15"/>
+    </row>
+    <row r="58" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A58" s="39" t="s">
         <v>125</v>
       </c>
@@ -8456,16 +9478,15 @@
       <c r="K58" s="28">
         <v>10834</v>
       </c>
-      <c r="L58" s="15"/>
-      <c r="M58" s="15"/>
-      <c r="N58" s="15"/>
-      <c r="O58" s="15">
+      <c r="L58" s="15">
         <f>C58/5</f>
         <v>1998.6</v>
       </c>
-      <c r="P58" s="15"/>
-    </row>
-    <row r="59" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="N58" s="15"/>
+      <c r="O58" s="15"/>
+      <c r="R58" s="15"/>
+    </row>
+    <row r="59" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A59" s="39" t="s">
         <v>124</v>
       </c>
@@ -8499,16 +9520,15 @@
       <c r="K59" s="28">
         <v>10897</v>
       </c>
-      <c r="L59" s="15"/>
-      <c r="M59" s="15"/>
+      <c r="L59" s="1">
+        <f>C58-L58</f>
+        <v>7994.4</v>
+      </c>
       <c r="N59" s="15"/>
-      <c r="O59" s="1">
-        <f>C58-O58</f>
-        <v>7994.4</v>
-      </c>
-      <c r="P59" s="15"/>
-    </row>
-    <row r="60" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="O59" s="15"/>
+      <c r="R59" s="15"/>
+    </row>
+    <row r="60" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A60" s="39" t="s">
         <v>123</v>
       </c>
@@ -8542,16 +9562,15 @@
       <c r="K60" s="28">
         <v>10909</v>
       </c>
-      <c r="L60" s="15"/>
-      <c r="M60" s="15"/>
-      <c r="N60" s="15"/>
-      <c r="O60" s="1">
+      <c r="L60" s="1">
         <f>+C59+C60</f>
         <v>20041</v>
       </c>
-      <c r="P60" s="15"/>
-    </row>
-    <row r="61" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="N60" s="15"/>
+      <c r="O60" s="15"/>
+      <c r="R60" s="15"/>
+    </row>
+    <row r="61" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A61" s="39" t="s">
         <v>122</v>
       </c>
@@ -8585,16 +9604,15 @@
       <c r="K61" s="28">
         <v>11026</v>
       </c>
-      <c r="L61" s="15"/>
-      <c r="M61" s="15"/>
-      <c r="N61" s="15"/>
-      <c r="O61" s="1">
+      <c r="L61" s="1">
         <f>+C61+C62</f>
         <v>21007</v>
       </c>
-      <c r="P61" s="15"/>
-    </row>
-    <row r="62" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="N61" s="15"/>
+      <c r="O61" s="15"/>
+      <c r="R61" s="15"/>
+    </row>
+    <row r="62" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A62" s="39" t="s">
         <v>121</v>
       </c>
@@ -8628,16 +9646,15 @@
       <c r="K62" s="28">
         <v>11453</v>
       </c>
-      <c r="L62" s="15"/>
-      <c r="M62" s="15"/>
-      <c r="N62" s="15"/>
-      <c r="O62" s="1">
+      <c r="L62" s="1">
         <f>+C63+C64</f>
         <v>22813</v>
       </c>
-      <c r="P62" s="15"/>
-    </row>
-    <row r="63" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="N62" s="15"/>
+      <c r="O62" s="15"/>
+      <c r="R62" s="15"/>
+    </row>
+    <row r="63" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A63" s="39" t="s">
         <v>120</v>
       </c>
@@ -8671,16 +9688,15 @@
       <c r="K63" s="28">
         <v>11975</v>
       </c>
-      <c r="L63" s="15"/>
-      <c r="M63" s="15"/>
-      <c r="N63" s="15"/>
-      <c r="O63" s="1">
+      <c r="L63" s="1">
         <f>+C65+C66</f>
         <v>21194</v>
       </c>
-      <c r="P63" s="15"/>
-    </row>
-    <row r="64" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="N63" s="15"/>
+      <c r="O63" s="15"/>
+      <c r="R63" s="15"/>
+    </row>
+    <row r="64" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A64" s="39" t="s">
         <v>119</v>
       </c>
@@ -8714,16 +9730,15 @@
       <c r="K64" s="28">
         <v>12358</v>
       </c>
-      <c r="L64" s="15"/>
-      <c r="M64" s="15"/>
-      <c r="N64" s="15"/>
-      <c r="O64" s="1">
+      <c r="L64" s="1">
         <f>+C67+C68</f>
         <v>20558</v>
       </c>
-      <c r="P64" s="15"/>
-    </row>
-    <row r="65" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="N64" s="15"/>
+      <c r="O64" s="15"/>
+      <c r="R64" s="15"/>
+    </row>
+    <row r="65" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A65" s="39" t="s">
         <v>118</v>
       </c>
@@ -8757,16 +9772,15 @@
       <c r="K65" s="28">
         <v>12521</v>
       </c>
-      <c r="L65" s="15"/>
-      <c r="M65" s="15"/>
-      <c r="N65" s="15"/>
-      <c r="O65" s="1">
+      <c r="L65" s="1">
         <f>+C69+C70</f>
         <v>22092</v>
       </c>
-      <c r="P65" s="15"/>
-    </row>
-    <row r="66" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="N65" s="15"/>
+      <c r="O65" s="15"/>
+      <c r="R65" s="15"/>
+    </row>
+    <row r="66" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A66" s="39" t="s">
         <v>117</v>
       </c>
@@ -8800,16 +9814,15 @@
       <c r="K66" s="28">
         <v>12423</v>
       </c>
-      <c r="L66" s="15"/>
-      <c r="M66" s="15"/>
-      <c r="N66" s="15"/>
-      <c r="O66" s="1">
+      <c r="L66" s="1">
         <f>+C71+C72</f>
         <v>17460</v>
       </c>
-      <c r="P66" s="15"/>
-    </row>
-    <row r="67" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="N66" s="15"/>
+      <c r="O66" s="15"/>
+      <c r="R66" s="15"/>
+    </row>
+    <row r="67" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A67" s="39" t="s">
         <v>116</v>
       </c>
@@ -8843,16 +9856,15 @@
       <c r="K67" s="28">
         <v>12175</v>
       </c>
-      <c r="L67" s="15"/>
-      <c r="M67" s="15"/>
-      <c r="N67" s="15"/>
-      <c r="O67" s="1">
+      <c r="L67" s="1">
         <f>+C73+C74</f>
         <v>9294</v>
       </c>
-      <c r="P67" s="15"/>
-    </row>
-    <row r="68" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="N67" s="15"/>
+      <c r="O67" s="15"/>
+      <c r="R67" s="15"/>
+    </row>
+    <row r="68" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A68" s="39" t="s">
         <v>115</v>
       </c>
@@ -8886,16 +9898,15 @@
       <c r="K68" s="28">
         <v>12234</v>
       </c>
-      <c r="L68" s="15"/>
-      <c r="M68" s="15"/>
-      <c r="N68" s="15"/>
-      <c r="O68" s="1">
+      <c r="L68" s="1">
         <f>+C75+C76+C77+C78</f>
         <v>4283</v>
       </c>
-      <c r="P68" s="15"/>
-    </row>
-    <row r="69" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="N68" s="15"/>
+      <c r="O68" s="15"/>
+      <c r="R68" s="15"/>
+    </row>
+    <row r="69" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A69" s="39" t="s">
         <v>114</v>
       </c>
@@ -8929,13 +9940,14 @@
       <c r="K69" s="28">
         <v>12011</v>
       </c>
-      <c r="L69" s="15"/>
+      <c r="L69" s="27"/>
       <c r="M69" s="15"/>
       <c r="N69" s="15"/>
       <c r="O69" s="15"/>
-      <c r="P69" s="15"/>
-    </row>
-    <row r="70" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="Q69" s="15"/>
+      <c r="R69" s="15"/>
+    </row>
+    <row r="70" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A70" s="39" t="s">
         <v>113</v>
       </c>
@@ -8969,13 +9981,14 @@
       <c r="K70" s="28">
         <v>11783</v>
       </c>
-      <c r="L70" s="15"/>
+      <c r="L70" s="27"/>
       <c r="M70" s="15"/>
       <c r="N70" s="15"/>
       <c r="O70" s="15"/>
-      <c r="P70" s="15"/>
-    </row>
-    <row r="71" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="Q70" s="15"/>
+      <c r="R70" s="15"/>
+    </row>
+    <row r="71" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A71" s="39" t="s">
         <v>112</v>
       </c>
@@ -9009,13 +10022,14 @@
       <c r="K71" s="28">
         <v>11727</v>
       </c>
-      <c r="L71" s="15"/>
+      <c r="L71" s="27"/>
       <c r="M71" s="15"/>
       <c r="N71" s="15"/>
       <c r="O71" s="15"/>
-      <c r="P71" s="15"/>
-    </row>
-    <row r="72" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="Q71" s="15"/>
+      <c r="R71" s="15"/>
+    </row>
+    <row r="72" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A72" s="39" t="s">
         <v>111</v>
       </c>
@@ -9049,13 +10063,14 @@
       <c r="K72" s="28">
         <v>10756</v>
       </c>
-      <c r="L72" s="15"/>
+      <c r="L72" s="27"/>
       <c r="M72" s="15"/>
       <c r="N72" s="15"/>
       <c r="O72" s="15"/>
-      <c r="P72" s="15"/>
-    </row>
-    <row r="73" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="Q72" s="15"/>
+      <c r="R72" s="15"/>
+    </row>
+    <row r="73" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A73" s="39" t="s">
         <v>110</v>
       </c>
@@ -9089,13 +10104,14 @@
       <c r="K73" s="28">
         <v>9410</v>
       </c>
-      <c r="L73" s="15"/>
+      <c r="L73" s="27"/>
       <c r="M73" s="15"/>
       <c r="N73" s="15"/>
       <c r="O73" s="15"/>
-      <c r="P73" s="15"/>
-    </row>
-    <row r="74" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="Q73" s="15"/>
+      <c r="R73" s="15"/>
+    </row>
+    <row r="74" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A74" s="39" t="s">
         <v>109</v>
       </c>
@@ -9129,13 +10145,14 @@
       <c r="K74" s="28">
         <v>7577</v>
       </c>
-      <c r="L74" s="15"/>
+      <c r="L74" s="27"/>
       <c r="M74" s="15"/>
       <c r="N74" s="15"/>
       <c r="O74" s="15"/>
-      <c r="P74" s="15"/>
-    </row>
-    <row r="75" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="Q74" s="15"/>
+      <c r="R74" s="15"/>
+    </row>
+    <row r="75" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A75" s="39" t="s">
         <v>108</v>
       </c>
@@ -9169,13 +10186,14 @@
       <c r="K75" s="28">
         <v>5680</v>
       </c>
-      <c r="L75" s="15"/>
+      <c r="L75" s="27"/>
       <c r="M75" s="15"/>
       <c r="N75" s="15"/>
       <c r="O75" s="15"/>
-      <c r="P75" s="15"/>
-    </row>
-    <row r="76" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="Q75" s="15"/>
+      <c r="R75" s="15"/>
+    </row>
+    <row r="76" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A76" s="39" t="s">
         <v>107</v>
       </c>
@@ -9209,13 +10227,14 @@
       <c r="K76" s="28">
         <v>3667</v>
       </c>
-      <c r="L76" s="15"/>
+      <c r="L76" s="27"/>
       <c r="M76" s="15"/>
       <c r="N76" s="15"/>
       <c r="O76" s="15"/>
-      <c r="P76" s="15"/>
-    </row>
-    <row r="77" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="Q76" s="15"/>
+      <c r="R76" s="15"/>
+    </row>
+    <row r="77" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A77" s="39" t="s">
         <v>106</v>
       </c>
@@ -9249,13 +10268,14 @@
       <c r="K77" s="28">
         <v>1773</v>
       </c>
-      <c r="L77" s="15"/>
+      <c r="L77" s="27"/>
       <c r="M77" s="15"/>
       <c r="N77" s="15"/>
       <c r="O77" s="15"/>
-      <c r="P77" s="15"/>
-    </row>
-    <row r="78" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="Q77" s="15"/>
+      <c r="R77" s="15"/>
+    </row>
+    <row r="78" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A78" s="47" t="s">
         <v>105</v>
       </c>
@@ -9289,13 +10309,14 @@
       <c r="K78" s="28">
         <v>422</v>
       </c>
-      <c r="L78" s="15"/>
+      <c r="L78" s="27"/>
       <c r="M78" s="15"/>
       <c r="N78" s="15"/>
       <c r="O78" s="15"/>
-      <c r="P78" s="15"/>
-    </row>
-    <row r="79" spans="1:29" s="21" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Q78" s="15"/>
+      <c r="R78" s="15"/>
+    </row>
+    <row r="79" spans="1:30" s="21" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" s="16" t="s">
         <v>104</v>
       </c>
@@ -9309,8 +10330,8 @@
       <c r="I79" s="31"/>
       <c r="J79" s="31"/>
       <c r="K79" s="31"/>
-      <c r="Q79" s="54"/>
-      <c r="R79" s="54"/>
+      <c r="L79" s="32"/>
+      <c r="P79" s="54"/>
       <c r="S79" s="54"/>
       <c r="T79" s="54"/>
       <c r="U79" s="54"/>
@@ -9322,10 +10343,10 @@
       <c r="AA79" s="54"/>
       <c r="AB79" s="54"/>
       <c r="AC79" s="54"/>
-    </row>
-    <row r="80" spans="1:29" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="Q80" s="54"/>
-      <c r="R80" s="54"/>
+      <c r="AD79" s="54"/>
+    </row>
+    <row r="80" spans="1:30" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="P80" s="54"/>
       <c r="S80" s="54"/>
       <c r="T80" s="54"/>
       <c r="U80" s="54"/>
@@ -9337,8 +10358,9 @@
       <c r="AA80" s="54"/>
       <c r="AB80" s="54"/>
       <c r="AC80" s="54"/>
-    </row>
-    <row r="81" spans="1:29" s="21" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AD80" s="54"/>
+    </row>
+    <row r="81" spans="1:30" s="21" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" s="46" t="s">
         <v>103</v>
       </c>
@@ -9352,8 +10374,8 @@
       <c r="I81" s="32"/>
       <c r="J81" s="32"/>
       <c r="K81" s="32"/>
-      <c r="Q81" s="54"/>
-      <c r="R81" s="54"/>
+      <c r="L81" s="32"/>
+      <c r="P81" s="54"/>
       <c r="S81" s="54"/>
       <c r="T81" s="54"/>
       <c r="U81" s="54"/>
@@ -9365,23 +10387,24 @@
       <c r="AA81" s="54"/>
       <c r="AB81" s="54"/>
       <c r="AC81" s="54"/>
-    </row>
-    <row r="82" spans="1:29" s="21" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A82" s="78" t="s">
+      <c r="AD81" s="54"/>
+    </row>
+    <row r="82" spans="1:30" s="21" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A82" s="81" t="s">
         <v>102</v>
       </c>
-      <c r="B82" s="79"/>
-      <c r="C82" s="79"/>
-      <c r="D82" s="79"/>
-      <c r="E82" s="79"/>
-      <c r="F82" s="79"/>
-      <c r="G82" s="79"/>
-      <c r="H82" s="79"/>
-      <c r="I82" s="79"/>
-      <c r="J82" s="79"/>
-      <c r="K82" s="79"/>
-      <c r="Q82" s="54"/>
-      <c r="R82" s="54"/>
+      <c r="B82" s="82"/>
+      <c r="C82" s="82"/>
+      <c r="D82" s="82"/>
+      <c r="E82" s="82"/>
+      <c r="F82" s="82"/>
+      <c r="G82" s="82"/>
+      <c r="H82" s="82"/>
+      <c r="I82" s="82"/>
+      <c r="J82" s="82"/>
+      <c r="K82" s="82"/>
+      <c r="L82" s="78"/>
+      <c r="P82" s="54"/>
       <c r="S82" s="54"/>
       <c r="T82" s="54"/>
       <c r="U82" s="54"/>
@@ -9393,8 +10416,9 @@
       <c r="AA82" s="54"/>
       <c r="AB82" s="54"/>
       <c r="AC82" s="54"/>
-    </row>
-    <row r="83" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AD82" s="54"/>
+    </row>
+    <row r="83" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B83" s="32"/>
       <c r="C83" s="32"/>
       <c r="D83" s="32"/>
@@ -9405,107 +10429,108 @@
       <c r="I83" s="32"/>
       <c r="J83" s="32"/>
       <c r="K83" s="32"/>
-    </row>
-    <row r="84" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L83" s="32"/>
+    </row>
+    <row r="84" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84" s="46" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="85" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" s="46" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="86" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A86" s="16" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="88" spans="1:29" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A88" s="80" t="s">
+    <row r="88" spans="1:30" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A88" s="83" t="s">
         <v>98</v>
       </c>
-      <c r="B88" s="81"/>
-      <c r="C88" s="81"/>
-      <c r="D88" s="81"/>
-      <c r="E88" s="81"/>
-      <c r="F88" s="81"/>
-      <c r="G88" s="81"/>
-      <c r="H88" s="81"/>
-      <c r="I88" s="79"/>
-    </row>
-    <row r="89" spans="1:29" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A89" s="80"/>
-      <c r="B89" s="81"/>
-      <c r="C89" s="81"/>
-      <c r="D89" s="81"/>
-      <c r="E89" s="81"/>
-      <c r="F89" s="81"/>
-      <c r="G89" s="81"/>
-      <c r="H89" s="81"/>
-      <c r="I89" s="79"/>
-    </row>
-    <row r="90" spans="1:29" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A90" s="80"/>
-      <c r="B90" s="81"/>
-      <c r="C90" s="81"/>
-      <c r="D90" s="81"/>
-      <c r="E90" s="81"/>
-      <c r="F90" s="81"/>
-      <c r="G90" s="81"/>
-      <c r="H90" s="81"/>
-      <c r="I90" s="79"/>
-    </row>
-    <row r="91" spans="1:29" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A91" s="80"/>
-      <c r="B91" s="81"/>
-      <c r="C91" s="81"/>
-      <c r="D91" s="81"/>
-      <c r="E91" s="81"/>
-      <c r="F91" s="81"/>
-      <c r="G91" s="81"/>
-      <c r="H91" s="81"/>
-      <c r="I91" s="79"/>
-    </row>
-    <row r="92" spans="1:29" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A92" s="80"/>
-      <c r="B92" s="81"/>
-      <c r="C92" s="81"/>
-      <c r="D92" s="81"/>
-      <c r="E92" s="81"/>
-      <c r="F92" s="81"/>
-      <c r="G92" s="81"/>
-      <c r="H92" s="81"/>
-      <c r="I92" s="79"/>
-    </row>
-    <row r="93" spans="1:29" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A93" s="81"/>
-      <c r="B93" s="81"/>
-      <c r="C93" s="81"/>
-      <c r="D93" s="81"/>
-      <c r="E93" s="81"/>
-      <c r="F93" s="81"/>
-      <c r="G93" s="81"/>
-      <c r="H93" s="81"/>
-      <c r="I93" s="79"/>
-    </row>
-    <row r="94" spans="1:29" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A94" s="81"/>
-      <c r="B94" s="81"/>
-      <c r="C94" s="81"/>
-      <c r="D94" s="81"/>
-      <c r="E94" s="81"/>
-      <c r="F94" s="81"/>
-      <c r="G94" s="81"/>
-      <c r="H94" s="81"/>
-      <c r="I94" s="79"/>
+      <c r="B88" s="84"/>
+      <c r="C88" s="84"/>
+      <c r="D88" s="84"/>
+      <c r="E88" s="84"/>
+      <c r="F88" s="84"/>
+      <c r="G88" s="84"/>
+      <c r="H88" s="84"/>
+      <c r="I88" s="82"/>
+    </row>
+    <row r="89" spans="1:30" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A89" s="83"/>
+      <c r="B89" s="84"/>
+      <c r="C89" s="84"/>
+      <c r="D89" s="84"/>
+      <c r="E89" s="84"/>
+      <c r="F89" s="84"/>
+      <c r="G89" s="84"/>
+      <c r="H89" s="84"/>
+      <c r="I89" s="82"/>
+    </row>
+    <row r="90" spans="1:30" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A90" s="83"/>
+      <c r="B90" s="84"/>
+      <c r="C90" s="84"/>
+      <c r="D90" s="84"/>
+      <c r="E90" s="84"/>
+      <c r="F90" s="84"/>
+      <c r="G90" s="84"/>
+      <c r="H90" s="84"/>
+      <c r="I90" s="82"/>
+    </row>
+    <row r="91" spans="1:30" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A91" s="83"/>
+      <c r="B91" s="84"/>
+      <c r="C91" s="84"/>
+      <c r="D91" s="84"/>
+      <c r="E91" s="84"/>
+      <c r="F91" s="84"/>
+      <c r="G91" s="84"/>
+      <c r="H91" s="84"/>
+      <c r="I91" s="82"/>
+    </row>
+    <row r="92" spans="1:30" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A92" s="83"/>
+      <c r="B92" s="84"/>
+      <c r="C92" s="84"/>
+      <c r="D92" s="84"/>
+      <c r="E92" s="84"/>
+      <c r="F92" s="84"/>
+      <c r="G92" s="84"/>
+      <c r="H92" s="84"/>
+      <c r="I92" s="82"/>
+    </row>
+    <row r="93" spans="1:30" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A93" s="84"/>
+      <c r="B93" s="84"/>
+      <c r="C93" s="84"/>
+      <c r="D93" s="84"/>
+      <c r="E93" s="84"/>
+      <c r="F93" s="84"/>
+      <c r="G93" s="84"/>
+      <c r="H93" s="84"/>
+      <c r="I93" s="82"/>
+    </row>
+    <row r="94" spans="1:30" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A94" s="84"/>
+      <c r="B94" s="84"/>
+      <c r="C94" s="84"/>
+      <c r="D94" s="84"/>
+      <c r="E94" s="84"/>
+      <c r="F94" s="84"/>
+      <c r="G94" s="84"/>
+      <c r="H94" s="84"/>
+      <c r="I94" s="82"/>
     </row>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="A1:K1"/>
     <mergeCell ref="A82:K82"/>
     <mergeCell ref="A88:I94"/>
-    <mergeCell ref="Q6:R6"/>
+    <mergeCell ref="S6:T6"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.24" bottom="0.24" header="0.2" footer="0.2"/>
   <pageSetup scale="65" orientation="portrait" r:id="rId1"/>

</xml_diff>